<commit_message>
Add phenomenon function운형 전처리 함수를 변형함
</commit_message>
<xml_diff>
--- a/docs/기상청_지상(종관,ASOS)시간자료_조회서비스_오픈API활용가이드.xlsx
+++ b/docs/기상청_지상(종관,ASOS)시간자료_조회서비스_오픈API활용가이드.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jongh.DESKTOP-HG781HU\OneDrive\open_api\weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D605408D-F1AA-4DAC-BA76-4380B4933E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AB00EFA-58A7-41FD-A238-2FB01247748E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{7B1E9A9E-4606-4B13-BDBD-5663744F4837}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="4" xr2:uid="{7B1E9A9E-4606-4B13-BDBD-5663744F4837}"/>
   </bookViews>
   <sheets>
     <sheet name="요청_메시지_명세" sheetId="5" r:id="rId1"/>
     <sheet name="응답_메시지_명세" sheetId="1" r:id="rId2"/>
     <sheet name="지점_코드" sheetId="2" r:id="rId3"/>
     <sheet name="플래그_종류(의미)" sheetId="4" r:id="rId4"/>
-    <sheet name="Open_API_에러_코드_정리" sheetId="3" r:id="rId5"/>
+    <sheet name="운형 약어" sheetId="6" r:id="rId5"/>
+    <sheet name="현상번호" sheetId="7" r:id="rId6"/>
+    <sheet name="Open_API_에러_코드_정리" sheetId="3" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">현상번호!$A$1:$J$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="423">
   <si>
     <t>항목명(국문)</t>
   </si>
@@ -1030,12 +1035,330 @@
     <t>공공데이터포털에서 발급받은 인증키(URL_Encode)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>권적운</t>
+  </si>
+  <si>
+    <t>권층운</t>
+  </si>
+  <si>
+    <t>Cirrus</t>
+  </si>
+  <si>
+    <t>Cirrocumulus</t>
+  </si>
+  <si>
+    <t>Cirrostratus</t>
+  </si>
+  <si>
+    <t>Ci</t>
+  </si>
+  <si>
+    <t>Cc</t>
+  </si>
+  <si>
+    <t>Cs</t>
+  </si>
+  <si>
+    <t>고적운</t>
+  </si>
+  <si>
+    <t>고층운</t>
+  </si>
+  <si>
+    <t>난층운</t>
+  </si>
+  <si>
+    <t>Altocumulus</t>
+  </si>
+  <si>
+    <t>Altostratus</t>
+  </si>
+  <si>
+    <t>Nimbostratus</t>
+  </si>
+  <si>
+    <t>Ac</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>Ns</t>
+  </si>
+  <si>
+    <t>층적운</t>
+  </si>
+  <si>
+    <t>Stratocumulus</t>
+  </si>
+  <si>
+    <t>Stratus</t>
+  </si>
+  <si>
+    <t>Sc</t>
+  </si>
+  <si>
+    <t>St</t>
+  </si>
+  <si>
+    <t>적란운</t>
+  </si>
+  <si>
+    <t>Cumulus</t>
+  </si>
+  <si>
+    <t>Cumulonimbus</t>
+  </si>
+  <si>
+    <t>Cu</t>
+  </si>
+  <si>
+    <t>Cb</t>
+  </si>
+  <si>
+    <t>층</t>
+  </si>
+  <si>
+    <t>약어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영문명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>명칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상층</t>
+  </si>
+  <si>
+    <t>권운</t>
+  </si>
+  <si>
+    <t>중층</t>
+  </si>
+  <si>
+    <t>하층</t>
+  </si>
+  <si>
+    <t>층운</t>
+  </si>
+  <si>
+    <t>적운</t>
+  </si>
+  <si>
+    <t>기호</t>
+  </si>
+  <si>
+    <t>기상현상</t>
+  </si>
+  <si>
+    <t>비</t>
+  </si>
+  <si>
+    <t>이슬비</t>
+  </si>
+  <si>
+    <t>소낙비</t>
+  </si>
+  <si>
+    <t>눈</t>
+  </si>
+  <si>
+    <t>진눈깨비</t>
+  </si>
+  <si>
+    <t>소낙눈</t>
+  </si>
+  <si>
+    <t>싸락눈</t>
+  </si>
+  <si>
+    <t>가루눈</t>
+  </si>
+  <si>
+    <t>어는비</t>
+  </si>
+  <si>
+    <t>싸락우박</t>
+  </si>
+  <si>
+    <t>얼음안개</t>
+  </si>
+  <si>
+    <t>먼지연무</t>
+  </si>
+  <si>
+    <t>높은날린먼지</t>
+  </si>
+  <si>
+    <t>먼지보라</t>
+  </si>
+  <si>
+    <t>아지랑이</t>
+  </si>
+  <si>
+    <t>놀</t>
+  </si>
+  <si>
+    <t>부분강수</t>
+  </si>
+  <si>
+    <t>맑음</t>
+  </si>
+  <si>
+    <t>구름조금</t>
+  </si>
+  <si>
+    <t>착빙성의이슬비</t>
+  </si>
+  <si>
+    <t>안개,낮은안개</t>
+  </si>
+  <si>
+    <t>박무</t>
+  </si>
+  <si>
+    <t>눈보라</t>
+  </si>
+  <si>
+    <t>서리</t>
+  </si>
+  <si>
+    <t>수상</t>
+  </si>
+  <si>
+    <t>우빙</t>
+  </si>
+  <si>
+    <t>해빙</t>
+  </si>
+  <si>
+    <t>연무</t>
+  </si>
+  <si>
+    <t>연기</t>
+  </si>
+  <si>
+    <t>햇무리</t>
+  </si>
+  <si>
+    <t>달코로나</t>
+  </si>
+  <si>
+    <t>어광</t>
+  </si>
+  <si>
+    <t>뇌전</t>
+  </si>
+  <si>
+    <t>세인트엘모의불</t>
+  </si>
+  <si>
+    <t>신적설</t>
+  </si>
+  <si>
+    <t>일조&lt;20%</t>
+  </si>
+  <si>
+    <t>우박</t>
+  </si>
+  <si>
+    <t>땅안개</t>
+  </si>
+  <si>
+    <t>땅날린눈</t>
+  </si>
+  <si>
+    <t>이슬</t>
+  </si>
+  <si>
+    <t>서릿발</t>
+  </si>
+  <si>
+    <t>수빙</t>
+  </si>
+  <si>
+    <t>결빙</t>
+  </si>
+  <si>
+    <t>유빙</t>
+  </si>
+  <si>
+    <t>강회</t>
+  </si>
+  <si>
+    <t>달무리</t>
+  </si>
+  <si>
+    <t>채운</t>
+  </si>
+  <si>
+    <t>비숍환</t>
+  </si>
+  <si>
+    <t>천둥</t>
+  </si>
+  <si>
+    <t>극광</t>
+  </si>
+  <si>
+    <t>일조≥80%</t>
+  </si>
+  <si>
+    <t>착빙성의비</t>
+  </si>
+  <si>
+    <t>소낙성진눈깨비</t>
+  </si>
+  <si>
+    <t>얼음침</t>
+  </si>
+  <si>
+    <t>높은날린눈</t>
+  </si>
+  <si>
+    <t>언이슬</t>
+  </si>
+  <si>
+    <t>무빙</t>
+  </si>
+  <si>
+    <t>조빙</t>
+  </si>
+  <si>
+    <t>용오름</t>
+  </si>
+  <si>
+    <t>해명</t>
+  </si>
+  <si>
+    <t>황사</t>
+  </si>
+  <si>
+    <t>땅날린먼지</t>
+  </si>
+  <si>
+    <t>회오리바람</t>
+  </si>
+  <si>
+    <t>해코로나</t>
+  </si>
+  <si>
+    <t>무지개</t>
+  </si>
+  <si>
+    <t>신기루</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1112,6 +1435,15 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1307,7 +1639,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1388,6 +1720,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1708,8 +2043,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -1976,7 +2311,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F45"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -4030,9 +4365,967 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62908604-34F8-469F-882A-6E6E3DF07ECF}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="5.0625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.4375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="C5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="C6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="C7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="C8" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A9" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="C9" t="s">
+        <v>353</v>
+      </c>
+      <c r="D9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A10" t="s">
+        <v>343</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="C10" t="s">
+        <v>354</v>
+      </c>
+      <c r="D10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="C11" t="s">
+        <v>340</v>
+      </c>
+      <c r="D11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24.75" x14ac:dyDescent="0.6">
+      <c r="A12"/>
+      <c r="B12" s="27"/>
+      <c r="C12"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63451F3A-24BD-488A-BE9F-2B422666EBFC}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:C68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="2" max="2" width="13.5625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>360</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>362</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>363</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>364</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>366</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>393</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>410</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>377</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>394</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>367</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>378</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>395</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>411</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>379</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>396</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>412</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>380</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>397</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>413</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>381</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>414</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>382</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>399</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>415</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>383</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>400</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>416</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A38">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>384</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A39">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>368</v>
+      </c>
+      <c r="C39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A40">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>417</v>
+      </c>
+      <c r="C40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A41">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>385</v>
+      </c>
+      <c r="C41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A42">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>401</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A43">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>418</v>
+      </c>
+      <c r="C43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A44">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>369</v>
+      </c>
+      <c r="C44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A45">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>370</v>
+      </c>
+      <c r="C45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>419</v>
+      </c>
+      <c r="C46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A47">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>386</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A48">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>402</v>
+      </c>
+      <c r="C48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A49">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>420</v>
+      </c>
+      <c r="C49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A50">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>387</v>
+      </c>
+      <c r="C50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A51">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>403</v>
+      </c>
+      <c r="C51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A52">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>421</v>
+      </c>
+      <c r="C52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A53">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>388</v>
+      </c>
+      <c r="C53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A54">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
+        <v>404</v>
+      </c>
+      <c r="C54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A55">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>422</v>
+      </c>
+      <c r="C55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A56">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>371</v>
+      </c>
+      <c r="C56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A57">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>372</v>
+      </c>
+      <c r="C57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A58">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>389</v>
+      </c>
+      <c r="C58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A59">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>405</v>
+      </c>
+      <c r="C59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A60">
+        <v>73</v>
+      </c>
+      <c r="B60" t="s">
+        <v>390</v>
+      </c>
+      <c r="C60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A61">
+        <v>74</v>
+      </c>
+      <c r="B61" t="s">
+        <v>406</v>
+      </c>
+      <c r="C61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A62">
+        <v>80</v>
+      </c>
+      <c r="B62" t="s">
+        <v>391</v>
+      </c>
+      <c r="C62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A63">
+        <v>81</v>
+      </c>
+      <c r="B63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A64">
+        <v>83</v>
+      </c>
+      <c r="B64" t="s">
+        <v>392</v>
+      </c>
+      <c r="C64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A65">
+        <v>84</v>
+      </c>
+      <c r="B65" t="s">
+        <v>407</v>
+      </c>
+      <c r="C65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A66">
+        <v>86</v>
+      </c>
+      <c r="B66" t="s">
+        <v>373</v>
+      </c>
+      <c r="C66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A67">
+        <v>90</v>
+      </c>
+      <c r="B67" t="s">
+        <v>374</v>
+      </c>
+      <c r="C67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A68">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
+        <v>375</v>
+      </c>
+      <c r="C68">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{63451F3A-24BD-488A-BE9F-2B422666EBFC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J68">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4ECA3C-04E4-4BE1-8A2A-8FD20698F2A2}">
   <sheetPr>
-    <tabColor rgb="FF00B050"/>
+    <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>

</xml_diff>